<commit_message>
R15 Updated Torque Curve 140215 Version
</commit_message>
<xml_diff>
--- a/R15EngineTorqueCurve.xlsx
+++ b/R15EngineTorqueCurve.xlsx
@@ -366,65 +366,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>4842</v>
+        <v>4324</v>
       </c>
       <c r="B1">
-        <v>34.031030545</v>
+        <v>34.16661234</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5102</v>
+        <v>4524</v>
       </c>
       <c r="B2">
-        <v>35.386848495000002</v>
+        <v>34.573357725000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5352</v>
+        <v>4771</v>
       </c>
       <c r="B3">
-        <v>37.827320804999999</v>
+        <v>35.929175675000003</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5558</v>
+        <v>5039</v>
       </c>
       <c r="B4">
-        <v>40.945702089999997</v>
+        <v>38.369647985</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5709</v>
+        <v>5297</v>
       </c>
       <c r="B5">
-        <v>43.792919784999995</v>
+        <v>41.623611064999999</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5818</v>
+        <v>5525</v>
       </c>
       <c r="B6">
-        <v>45.691064915000005</v>
+        <v>44.470828759999996</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5907</v>
+        <v>5712</v>
       </c>
       <c r="B7">
         <v>46.64013748</v>
@@ -432,751 +432,543 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5994</v>
+        <v>5861</v>
       </c>
       <c r="B8">
-        <v>46.64013748</v>
+        <v>47.860373634999995</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6092</v>
+        <v>5986</v>
       </c>
       <c r="B9">
-        <v>46.368973890000007</v>
+        <v>48.131537225000002</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6200</v>
+        <v>6101</v>
       </c>
       <c r="B10">
-        <v>45.962228504999999</v>
+        <v>47.860373634999995</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6318</v>
+        <v>6225</v>
       </c>
       <c r="B11">
-        <v>45.555483120000005</v>
+        <v>47.589210045000002</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>6439</v>
+        <v>6368</v>
       </c>
       <c r="B12">
-        <v>45.013155940000004</v>
+        <v>47.046882865000008</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>6564</v>
+        <v>6544</v>
       </c>
       <c r="B13">
-        <v>44.470828759999996</v>
+        <v>46.504555685</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>6701</v>
+        <v>6761</v>
       </c>
       <c r="B14">
-        <v>44.064083375000003</v>
+        <v>45.962228504999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>6863</v>
+        <v>7016</v>
       </c>
       <c r="B15">
-        <v>43.928501580000002</v>
+        <v>45.826646709999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>7063</v>
+        <v>7296</v>
       </c>
       <c r="B16">
-        <v>44.335246965000003</v>
+        <v>46.368973890000007</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>7300</v>
+        <v>7587</v>
       </c>
       <c r="B17">
-        <v>45.555483120000005</v>
+        <v>47.724791840000009</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>7563</v>
+        <v>7868</v>
       </c>
       <c r="B18">
-        <v>47.182464660000001</v>
+        <v>49.487355175000005</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>7833</v>
+        <v>8126</v>
       </c>
       <c r="B19">
-        <v>49.216191584999997</v>
+        <v>51.521082100000001</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>8088</v>
+        <v>8346</v>
       </c>
       <c r="B20">
-        <v>50.978754920000007</v>
+        <v>53.419227229999997</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>8311</v>
+        <v>8523</v>
       </c>
       <c r="B21">
-        <v>52.334572870000002</v>
+        <v>54.775045179999999</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>8488</v>
+        <v>8661</v>
       </c>
       <c r="B22">
-        <v>53.148063640000004</v>
+        <v>55.588535950000001</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>8616</v>
+        <v>8770</v>
       </c>
       <c r="B23">
-        <v>53.825972615000005</v>
+        <v>55.995281335000001</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>8705</v>
+        <v>8865</v>
       </c>
       <c r="B24">
-        <v>54.097136204999998</v>
+        <v>56.130863130000002</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>8765</v>
+        <v>8955</v>
       </c>
       <c r="B25">
-        <v>54.232718000000006</v>
+        <v>56.130863130000002</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>8810</v>
+        <v>9043</v>
       </c>
       <c r="B26">
-        <v>54.232718000000006</v>
+        <v>56.130863130000002</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>8848</v>
+        <v>9128</v>
       </c>
       <c r="B27">
-        <v>54.232718000000006</v>
+        <v>55.995281335000001</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>8880</v>
+        <v>9209</v>
       </c>
       <c r="B28">
-        <v>54.097136204999998</v>
+        <v>55.724117745000001</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>8910</v>
+        <v>9287</v>
       </c>
       <c r="B29">
-        <v>53.961554409999998</v>
+        <v>55.588535950000001</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>8936</v>
+        <v>9363</v>
       </c>
       <c r="B30">
-        <v>53.825972615000005</v>
+        <v>55.31737236</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>8960</v>
+        <v>9440</v>
       </c>
       <c r="B31">
-        <v>53.690390820000005</v>
+        <v>55.046208770000007</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>8983</v>
+        <v>9517</v>
       </c>
       <c r="B32">
-        <v>53.554809025000004</v>
+        <v>54.775045179999999</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>9008</v>
+        <v>9595</v>
       </c>
       <c r="B33">
-        <v>53.419227229999997</v>
+        <v>54.503881590000006</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>9036</v>
+        <v>9671</v>
       </c>
       <c r="B34">
-        <v>53.283645434999997</v>
+        <v>54.097136204999998</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>9069</v>
+        <v>9741</v>
       </c>
       <c r="B35">
-        <v>53.148063640000004</v>
+        <v>53.690390820000005</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>9104</v>
+        <v>9803</v>
       </c>
       <c r="B36">
-        <v>53.012481845000003</v>
+        <v>53.283645434999997</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>9141</v>
+        <v>9859</v>
       </c>
       <c r="B37">
-        <v>52.876900050000003</v>
+        <v>52.741318255000003</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>9177</v>
+        <v>9913</v>
       </c>
       <c r="B38">
-        <v>52.876900050000003</v>
+        <v>52.334572870000002</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>9213</v>
+        <v>9967</v>
       </c>
       <c r="B39">
-        <v>52.741318255000003</v>
+        <v>51.792245690000009</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>9250</v>
+        <v>10024</v>
       </c>
       <c r="B40">
-        <v>52.605736459999996</v>
+        <v>51.114336715000007</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>9286</v>
+        <v>10086</v>
       </c>
       <c r="B41">
-        <v>52.605736459999996</v>
+        <v>50.436427740000006</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>9323</v>
+        <v>10155</v>
       </c>
       <c r="B42">
-        <v>52.470154665000003</v>
+        <v>49.758518765000005</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>9361</v>
+        <v>10241</v>
       </c>
       <c r="B43">
-        <v>52.334572870000002</v>
+        <v>49.080609790000004</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>9397</v>
+        <v>10347</v>
       </c>
       <c r="B44">
-        <v>52.198991075000002</v>
+        <v>48.538282609999996</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>9434</v>
+        <v>10474</v>
       </c>
       <c r="B45">
-        <v>52.198991075000002</v>
+        <v>48.131537225000002</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>9469</v>
+        <v>10614</v>
       </c>
       <c r="B46">
-        <v>52.063409280000002</v>
+        <v>47.860373634999995</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>9505</v>
+        <v>10758</v>
       </c>
       <c r="B47">
-        <v>51.927827484999995</v>
+        <v>47.589210045000002</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>9545</v>
+        <v>10897</v>
       </c>
       <c r="B48">
-        <v>51.927827484999995</v>
+        <v>47.318046455000001</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>9584</v>
+        <v>11026</v>
       </c>
       <c r="B49">
-        <v>51.927827484999995</v>
+        <v>46.91130107</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>9624</v>
+        <v>11146</v>
       </c>
       <c r="B50">
-        <v>51.927827484999995</v>
+        <v>46.504555685</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>9659</v>
+        <v>11259</v>
       </c>
       <c r="B51">
-        <v>51.927827484999995</v>
+        <v>45.962228504999999</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>9693</v>
+        <v>11369</v>
       </c>
       <c r="B52">
-        <v>51.927827484999995</v>
+        <v>45.419901325000005</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>9725</v>
+        <v>11479</v>
       </c>
       <c r="B53">
-        <v>51.792245690000009</v>
+        <v>44.606410554999997</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>9755</v>
+        <v>11588</v>
       </c>
       <c r="B54">
-        <v>51.792245690000009</v>
+        <v>43.792919784999995</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>9785</v>
+        <v>11696</v>
       </c>
       <c r="B55">
-        <v>51.656663895000001</v>
+        <v>42.843847220000001</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>9812</v>
+        <v>11791</v>
       </c>
       <c r="B56">
-        <v>51.656663895000001</v>
+        <v>41.623611064999999</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>9838</v>
+        <v>11866</v>
       </c>
       <c r="B57">
-        <v>51.521082100000001</v>
+        <v>40.403374910000004</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>9864</v>
+        <v>11914</v>
       </c>
       <c r="B58">
-        <v>51.385500305000001</v>
+        <v>38.911975165000001</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>9893</v>
+        <v>11940</v>
       </c>
       <c r="B59">
-        <v>51.385500305000001</v>
+        <v>37.149411829999998</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>9926</v>
+        <v>11956</v>
       </c>
       <c r="B60">
-        <v>51.114336715000007</v>
+        <v>35.115684905000002</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>9962</v>
+        <v>11970</v>
       </c>
       <c r="B61">
-        <v>50.978754920000007</v>
+        <v>33.081957979999999</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>9998</v>
+        <v>11985</v>
       </c>
       <c r="B62">
-        <v>50.70759133</v>
+        <v>30.912649260000002</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>10031</v>
+        <v>12001</v>
       </c>
       <c r="B63">
-        <v>50.436427740000006</v>
+        <v>28.878922335000002</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>10063</v>
+        <v>12015</v>
       </c>
       <c r="B64">
-        <v>50.165264149999999</v>
+        <v>26.845195410000002</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>10093</v>
+        <v>12028</v>
       </c>
       <c r="B65">
-        <v>49.758518765000005</v>
+        <v>24.947050279999999</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>10123</v>
+        <v>12044</v>
       </c>
       <c r="B66">
-        <v>49.351773379999997</v>
+        <v>23.184486945000003</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>10155</v>
+        <v>12063</v>
       </c>
       <c r="B67">
-        <v>48.945027995000004</v>
+        <v>21.557505405000001</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>10190</v>
+        <v>12081</v>
       </c>
       <c r="B68">
-        <v>48.673864405000003</v>
+        <v>19.930523865000001</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>10230</v>
+        <v>12094</v>
       </c>
       <c r="B69">
-        <v>48.267119020000003</v>
+        <v>18.439124119999999</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>10272</v>
+        <v>12101</v>
       </c>
       <c r="B70">
-        <v>47.995955430000002</v>
+        <v>16.81214258</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>10320</v>
+        <v>12104</v>
       </c>
       <c r="B71">
-        <v>47.724791840000009</v>
+        <v>15.185161039999999</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>10374</v>
+        <v>12109</v>
       </c>
       <c r="B72">
-        <v>47.453628250000001</v>
+        <v>13.693761295</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>10435</v>
+        <v>12118</v>
       </c>
       <c r="B73">
-        <v>47.318046455000001</v>
+        <v>12.47352514</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>10500</v>
+        <v>12128</v>
       </c>
       <c r="B74">
-        <v>47.046882865000008</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>10567</v>
-      </c>
-      <c r="B75">
-        <v>46.775719275</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>10636</v>
-      </c>
-      <c r="B76">
-        <v>46.504555685</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>10706</v>
-      </c>
-      <c r="B77">
-        <v>46.233392095000006</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>10779</v>
-      </c>
-      <c r="B78">
-        <v>45.962228504999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>10855</v>
-      </c>
-      <c r="B79">
-        <v>45.691064915000005</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>10932</v>
-      </c>
-      <c r="B80">
-        <v>45.555483120000005</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>11010</v>
-      </c>
-      <c r="B81">
-        <v>45.284319529999998</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>11087</v>
-      </c>
-      <c r="B82">
-        <v>45.148737734999997</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>11165</v>
-      </c>
-      <c r="B83">
-        <v>44.877574145000004</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>11242</v>
-      </c>
-      <c r="B84">
-        <v>44.606410554999997</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>11318</v>
-      </c>
-      <c r="B85">
-        <v>44.335246965000003</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>11398</v>
-      </c>
-      <c r="B86">
-        <v>43.792919784999995</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>11484</v>
-      </c>
-      <c r="B87">
-        <v>43.250592605000001</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>11579</v>
-      </c>
-      <c r="B88">
-        <v>42.57268363</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>11677</v>
-      </c>
-      <c r="B89">
-        <v>41.894774654999999</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>11768</v>
-      </c>
-      <c r="B90">
-        <v>40.810120295000004</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>11846</v>
-      </c>
-      <c r="B91">
-        <v>39.589884140000002</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>11904</v>
-      </c>
-      <c r="B92">
-        <v>37.9629026</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>11943</v>
-      </c>
-      <c r="B93">
-        <v>36.200339265000004</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>11969</v>
-      </c>
-      <c r="B94">
-        <v>34.031030545</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>11984</v>
-      </c>
-      <c r="B95">
-        <v>31.72614003</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>11997</v>
-      </c>
-      <c r="B96">
-        <v>29.421249515</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>12010</v>
-      </c>
-      <c r="B97">
-        <v>27.116359000000003</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>12024</v>
-      </c>
-      <c r="B98">
-        <v>25.082632074999999</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>12038</v>
-      </c>
-      <c r="B99">
-        <v>23.184486945000003</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>12045</v>
-      </c>
-      <c r="B100">
-        <v>21.828668995000001</v>
+        <v>11.66003437</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B100">
-    <sortCondition ref="A1:A100"/>
+  <sortState ref="A1:B74">
+    <sortCondition ref="A1:A74"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>